<commit_message>
all features currently working
</commit_message>
<xml_diff>
--- a/missed_dates.xlsx
+++ b/missed_dates.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="35">
   <si>
     <t>Work Order Number</t>
   </si>
@@ -22,247 +22,79 @@
     <t>Sweeping Subs</t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 1/1, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
+    <t/>
   </si>
   <si>
     <t>Hazel</t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 1/11, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/25, 1/1, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 1/1, 1/16, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 1/16, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/30, 1/27, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 1/1, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 1/2, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 12/26, 1/1, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/26, 1/2, 1/27, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
     <t>Asphalt Maintenance</t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/28, 12/30, 12/31, 1/1, 1/2, 1/4, 1/6, 1/7, 1/8, 1/9, 1/11, 1/13, 1/14, 1/15, 1/16, 1/20, 1/21, 1/22, 1/23, 1/25, 1/27, 1/28, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/28, 12/30, 1/16, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/26, 1/5, 1/7, 1/12, 1/17, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/26, 1/7, 1/16, 1/20, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 1/1, 1/7, 1/16, 1/17, 1/21, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 1/7, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/28, 1/7, 1/16, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/28, 1/4, 1/7, 1/9, 1/11, 1/13, 1/16, 1/18, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/28, 1/16, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/26, 1/7, 1/10, 1/16, 1/17, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/30, 12/31, 1/1, 1/2, 1/4, 1/6, 1/7, 1/8, 1/9, 1/13, 1/15, 1/16, 1/20, 1/21, 1/22, 1/23, 1/25, 1/27, 1/28, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/30, 1/16, 1/20, 1/30, 2/3, 2/6</t>
+    <t>2/4</t>
   </si>
   <si>
     <t>east coast sweeping</t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/28, 1/6, 1/16, 1/20, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 1/16, 1/20, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/30, 1/16, 1/20, 1/23, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/31, 1/2, 1/4, 1/7, 1/9, 1/14, 1/16, 1/18, 1/21, 1/23, 1/25, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
+    <t>1/30, 2/1, 2/4, 2/11</t>
   </si>
   <si>
     <t>Marventanos</t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/31, 1/2, 1/4, 1/7, 1/9, 1/14, 1/16, 1/18, 1/20, 1/21, 1/23, 1/25, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/28, 12/31, 1/2, 1/4, 1/7, 1/9, 1/14, 1/16, 1/18, 1/21, 1/23, 1/25, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 1/16, 1/20, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
     <t>Madison Group</t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 1/2, 1/16, 1/20, 1/25, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/28, 12/30, 1/6, 1/9, 1/11, 1/13, 1/16, 1/18, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
+    <t>1/30, 2/1, 2/3</t>
   </si>
   <si>
     <t>Troiano</t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/30, 1/6, 1/9, 1/13, 1/16, 1/20, 1/23, 1/27, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/26, 12/30, 1/2, 1/6, 1/9, 1/13, 1/16, 1/20, 1/23, 1/27, 1/30, 2/3, 2/6</t>
+    <t>1/30, 2/3</t>
+  </si>
+  <si>
+    <t>2/3</t>
   </si>
   <si>
     <t>By Us ??</t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 1/1, 1/7, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
+    <t>1/29</t>
   </si>
   <si>
     <t xml:space="preserve">GJM </t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 1/1, 1/7, 1/8, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 1/1, 1/7, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 1/7, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 1/7, 1/30, 2/1, 2/3, 2/4, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 1/16, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
     <t>Area Sweeping</t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/30, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 1/2, 1/7, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 1/11, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/30, 1/18, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 1/7, 1/9, 1/14, 1/16, 1/18, 1/20, 1/23, 1/25, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coastal </t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 1/9, 1/16, 1/18, 1/20, 1/23, 1/25, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/28, 12/30, 1/2, 1/4, 1/6, 1/7, 1/9, 1/11, 1/13, 1/14, 1/16, 1/18, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/26, 1/9, 1/16, 1/20, 1/23, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 1/9, 1/13, 1/16, 1/18, 1/20, 1/23, 1/25, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 12/26, 1/1, 1/5, 1/7, 1/8, 1/9, 1/14, 1/15, 1/16, 1/17, 1/18, 1/20, 1/22, 1/23, 1/24, 1/25, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/28, 1/9, 1/13, 1/16, 1/18, 1/20, 1/23, 1/25, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 1/7, 1/16, 1/21, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
+    <t>2/11</t>
   </si>
   <si>
     <t>Martorelli</t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/25, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/31, 1/7, 1/14, 1/21, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 1/16, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 1/7, 1/21, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/28, 12/30, 1/4, 1/6, 1/7, 1/11, 1/13, 1/14, 1/18, 1/21, 1/28, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 12/26, 12/27, 1/1, 1/7, 1/8, 1/14, 1/16, 1/17, 1/21, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/28, 12/30, 1/2, 1/6, 1/9, 1/13, 1/16, 1/18, 1/20, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
+    <t>2/4, 2/11</t>
+  </si>
+  <si>
+    <t>1/29, 2/2</t>
+  </si>
+  <si>
+    <t>1/30, 2/1</t>
   </si>
   <si>
     <t>Split</t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/26, 12/30, 1/2, 1/6, 1/9, 1/13, 1/16, 1/20, 1/27, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/2, 1/6, 1/9, 1/13, 1/16, 1/18, 1/20, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/28, 12/30, 1/2, 1/4, 1/6, 1/9, 1/11, 1/13, 1/16, 1/18, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
+    <t>1/30</t>
+  </si>
+  <si>
+    <t>2/1, 2/3</t>
   </si>
   <si>
     <t>Always Growing</t>
@@ -277,55 +109,10 @@
     <t>Tom Vangordon/Precision snow</t>
   </si>
   <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/30, 1/4, 1/6, 1/8, 1/13, 1/14, 1/16, 1/20, 1/21, 1/25, 1/27, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/30, 1/4, 1/6, 1/7, 1/8, 1/9, 1/13, 1/15, 1/16, 1/18, 1/20, 1/21, 1/25, 1/27, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/28, 12/30, 1/4, 1/6, 1/7, 1/8, 1/13, 1/15, 1/16, 1/18, 1/20, 1/21, 1/25, 1/27, 1/28, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/28, 12/30, 1/4, 1/6, 1/7, 1/8, 1/13, 1/15, 1/16, 1/20, 1/22, 1/25, 1/27, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/30, 1/2, 1/4, 1/6, 1/7, 1/9, 1/13, 1/16, 1/18, 1/20, 1/21, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/2, 1/4, 1/6, 1/9, 1/11, 1/13, 1/16, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/4, 1/6, 1/9, 1/11, 1/13, 1/16, 1/20, 1/23, 1/25, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/2, 1/4, 1/6, 1/9, 1/11, 1/13, 1/16, 1/18, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/11, 12/12, 12/14, 12/16, 12/17, 12/18, 12/19, 12/21, 12/23, 12/24, 12/25, 12/26, 12/30, 1/4, 1/6, 1/7, 1/8, 1/13, 1/14, 1/15, 1/16, 1/18, 1/20, 1/21, 1/25, 1/27, 1/29, 1/30, 2/1, 2/3, 2/4, 2/5, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 12/30, 1/4, 1/6, 1/9, 1/11, 1/13, 1/16, 1/20, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/10, 12/12, 12/14, 12/16, 12/17, 12/19, 12/21, 12/23, 12/24, 12/26, 12/28, 1/2, 1/4, 1/7, 1/9, 1/11, 1/16, 1/18, 1/21, 1/23, 1/25, 1/27, 1/30, 2/1, 2/3, 2/4, 2/6, 2/8</t>
-  </si>
-  <si>
     <t xml:space="preserve">first choice   </t>
   </si>
   <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/26, 1/16, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 12/26, 1/13, 1/16, 1/20, 1/30, 2/3, 2/6</t>
-  </si>
-  <si>
-    <t>12/8, 12/9, 12/10, 12/11, 12/12, 12/13, 12/14, 12/15, 12/16, 12/17, 12/18, 12/19, 12/20, 12/21, 12/22, 12/23, 12/24, 12/25, 12/26, 1/1, 1/7, 1/8, 1/10, 1/17, 1/21, 1/24, 1/27, 1/29, 1/30, 1/31, 2/1, 2/2, 2/3, 2/4, 2/5, 2/6, 2/7, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/14, 12/16, 12/19, 12/21, 12/23, 12/26, 1/9, 1/16, 1/30, 2/1, 2/3, 2/6, 2/8</t>
-  </si>
-  <si>
-    <t>12/9, 12/12, 12/16, 12/19, 12/23, 1/2, 1/30, 2/3, 2/6</t>
+    <t>1/29, 2/3</t>
   </si>
   <si>
     <t>Dirtworks</t>
@@ -725,7 +512,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>264389601</v>
+        <v>267468036</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -736,10 +523,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>264389602</v>
+        <v>267468037</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -747,10 +534,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>264389604</v>
+        <v>267468039</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -758,7 +545,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>264389605</v>
+        <v>267468040</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -769,10 +556,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>264389606</v>
+        <v>267468041</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -780,10 +567,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>264389607</v>
+        <v>267468042</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -791,7 +578,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>264389608</v>
+        <v>267468043</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -802,10 +589,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>264389610</v>
+        <v>267468045</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -813,10 +600,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>264389611</v>
+        <v>267468046</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -824,10 +611,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>264389612</v>
+        <v>267468047</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -835,10 +622,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>264389613</v>
+        <v>267468048</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -846,10 +633,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>264389617</v>
+        <v>267468052</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -857,10 +644,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>264389618</v>
+        <v>267468053</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -868,7 +655,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>264389619</v>
+        <v>267468054</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -879,10 +666,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>264389620</v>
+        <v>267468055</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -890,10 +677,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>264389621</v>
+        <v>267468056</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -901,10 +688,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>264389623</v>
+        <v>267468058</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -912,10 +699,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>264389624</v>
+        <v>267468059</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -923,10 +710,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>264389625</v>
+        <v>267468060</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -934,10 +721,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>264389626</v>
+        <v>267468061</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -945,10 +732,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>264389773</v>
+        <v>267468208</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -956,10 +743,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>264389774</v>
+        <v>267468209</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -967,10 +754,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>264389775</v>
+        <v>267468210</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -978,10 +765,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>264389776</v>
+        <v>267468211</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -989,1333 +776,1333 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>264389777</v>
+        <v>267468212</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>264389603</v>
+        <v>267468038</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>264389778</v>
+        <v>267468213</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>264389609</v>
+        <v>267468044</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>264389614</v>
+        <v>267468049</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>264389615</v>
+        <v>267468050</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>264389781</v>
+        <v>267468216</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>264389782</v>
+        <v>267468217</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>264389783</v>
+        <v>267468218</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>264389784</v>
+        <v>267468219</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>264389785</v>
+        <v>267468220</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>264389788</v>
+        <v>267468223</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>264389772</v>
+        <v>267468207</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>264389789</v>
+        <v>267468224</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>264389779</v>
+        <v>267468214</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>264389780</v>
+        <v>267468215</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>264389786</v>
+        <v>267468221</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>264389787</v>
+        <v>267468222</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>264389616</v>
+        <v>267468051</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>264389622</v>
+        <v>267468057</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>264389627</v>
+        <v>267468062</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>264389790</v>
+        <v>267468225</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>264389791</v>
+        <v>267468226</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>264389792</v>
+        <v>267468227</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>264389793</v>
+        <v>267468228</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>264389794</v>
+        <v>267468229</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>264389795</v>
+        <v>267468230</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>264388899</v>
+        <v>267467838</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>264388900</v>
+        <v>267467839</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>264388901</v>
+        <v>267467840</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>264388902</v>
+        <v>267467841</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>264388906</v>
+        <v>267467845</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>264388907</v>
+        <v>267467846</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>264388903</v>
+        <v>267467842</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>264388904</v>
+        <v>267467843</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>264388905</v>
+        <v>267467844</v>
       </c>
       <c r="B61" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>264389556</v>
+        <v>267467991</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C62" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>264389796</v>
+        <v>267468231</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>264389799</v>
+        <v>267468234</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>264389804</v>
+        <v>267468239</v>
       </c>
       <c r="B65" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>264389808</v>
+        <v>267468243</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>264389815</v>
+        <v>267468250</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C67" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>264389816</v>
+        <v>267468251</v>
       </c>
       <c r="B68" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>264389817</v>
+        <v>267468252</v>
       </c>
       <c r="B69" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>264389820</v>
+        <v>267468255</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>264389822</v>
+        <v>267468257</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>264389823</v>
+        <v>267468258</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>264389828</v>
+        <v>267468263</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>264389830</v>
+        <v>267468265</v>
       </c>
       <c r="B74" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>264389831</v>
+        <v>267468266</v>
       </c>
       <c r="B75" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>264389557</v>
+        <v>267467992</v>
       </c>
       <c r="B76" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>264389558</v>
+        <v>267467993</v>
       </c>
       <c r="B77" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>264389559</v>
+        <v>267467994</v>
       </c>
       <c r="B78" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>264389560</v>
+        <v>267467995</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>264389561</v>
+        <v>267467996</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>264389565</v>
+        <v>267468000</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>264389566</v>
+        <v>267468001</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>264389567</v>
+        <v>267468002</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>264389568</v>
+        <v>267468003</v>
       </c>
       <c r="B84" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>264389569</v>
+        <v>267468004</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>264389570</v>
+        <v>267468005</v>
       </c>
       <c r="B86" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>264389571</v>
+        <v>267468006</v>
       </c>
       <c r="B87" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C87" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>264389600</v>
+        <v>267468035</v>
       </c>
       <c r="B88" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>264389797</v>
+        <v>267468232</v>
       </c>
       <c r="B89" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>264389801</v>
+        <v>267468236</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>264389803</v>
+        <v>267468238</v>
       </c>
       <c r="B91" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>264389809</v>
+        <v>267468244</v>
       </c>
       <c r="B92" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>264389819</v>
+        <v>267468254</v>
       </c>
       <c r="B93" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>264389824</v>
+        <v>267468259</v>
       </c>
       <c r="B94" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>264389826</v>
+        <v>267468261</v>
       </c>
       <c r="B95" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>264389798</v>
+        <v>267468233</v>
       </c>
       <c r="B96" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>264389805</v>
+        <v>267468240</v>
       </c>
       <c r="B97" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="C97" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>264389810</v>
+        <v>267468245</v>
       </c>
       <c r="B98" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="C98" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>264389821</v>
+        <v>267468256</v>
       </c>
       <c r="B99" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="C99" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>264389572</v>
+        <v>267468007</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C100" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>264389573</v>
+        <v>267468008</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>264389574</v>
+        <v>267468009</v>
       </c>
       <c r="B102" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>264389575</v>
+        <v>267468010</v>
       </c>
       <c r="B103" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>264389576</v>
+        <v>267468011</v>
       </c>
       <c r="B104" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="C104" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>264389577</v>
+        <v>267468012</v>
       </c>
       <c r="B105" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>264389586</v>
+        <v>267468021</v>
       </c>
       <c r="B106" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C106" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>264389800</v>
+        <v>267468235</v>
       </c>
       <c r="B107" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="C107" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>264389807</v>
+        <v>267468242</v>
       </c>
       <c r="B108" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>264389811</v>
+        <v>267468246</v>
       </c>
       <c r="B109" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>264389813</v>
+        <v>267468248</v>
       </c>
       <c r="B110" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>264389814</v>
+        <v>267468249</v>
       </c>
       <c r="B111" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>264389818</v>
+        <v>267468253</v>
       </c>
       <c r="B112" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="C112" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>264389827</v>
+        <v>267468262</v>
       </c>
       <c r="B113" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>264389832</v>
+        <v>267468267</v>
       </c>
       <c r="B114" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="C114" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>264389835</v>
+        <v>267468270</v>
       </c>
       <c r="B115" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="C115" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>264389802</v>
+        <v>267468237</v>
       </c>
       <c r="B116" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C116" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>264389806</v>
+        <v>267468241</v>
       </c>
       <c r="B117" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="C117" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>264389812</v>
+        <v>267468247</v>
       </c>
       <c r="B118" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C118" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>264389825</v>
+        <v>267468260</v>
       </c>
       <c r="B119" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C119" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>264389833</v>
+        <v>267468268</v>
       </c>
       <c r="B120" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="C120" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>264389834</v>
+        <v>267468269</v>
       </c>
       <c r="B121" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C121" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>264389829</v>
+        <v>267468264</v>
       </c>
       <c r="B122" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="C122" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>264389562</v>
+        <v>267467997</v>
       </c>
       <c r="B123" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>264389564</v>
+        <v>267467999</v>
       </c>
       <c r="B124" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>264389563</v>
+        <v>267467998</v>
       </c>
       <c r="B125" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C125" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>264389578</v>
+        <v>267468013</v>
       </c>
       <c r="B126" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C126" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>264389579</v>
+        <v>267468014</v>
       </c>
       <c r="B127" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="C127" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>264389580</v>
+        <v>267468015</v>
       </c>
       <c r="B128" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="C128" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>264389583</v>
+        <v>267468018</v>
       </c>
       <c r="B129" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="C129" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>264389584</v>
+        <v>267468019</v>
       </c>
       <c r="B130" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="C130" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>264389585</v>
+        <v>267468020</v>
       </c>
       <c r="B131" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="C131" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>264389589</v>
+        <v>267468024</v>
       </c>
       <c r="B132" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="C132" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>264389590</v>
+        <v>267468025</v>
       </c>
       <c r="B133" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="C133" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>264389596</v>
+        <v>267468031</v>
       </c>
       <c r="B134" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="C134" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>264389597</v>
+        <v>267468032</v>
       </c>
       <c r="B135" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="C135" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>264389598</v>
+        <v>267468033</v>
       </c>
       <c r="B136" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="C136" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>264389581</v>
+        <v>267468016</v>
       </c>
       <c r="B137" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="C137" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>264389582</v>
+        <v>267468017</v>
       </c>
       <c r="B138" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C138" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>264389587</v>
+        <v>267468022</v>
       </c>
       <c r="B139" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="C139" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>264389588</v>
+        <v>267468023</v>
       </c>
       <c r="B140" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="C140" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>264389591</v>
+        <v>267468026</v>
       </c>
       <c r="B141" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="C141" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>264389592</v>
+        <v>267468027</v>
       </c>
       <c r="B142" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="C142" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>264389593</v>
+        <v>267468028</v>
       </c>
       <c r="B143" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="C143" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>264389594</v>
+        <v>267468029</v>
       </c>
       <c r="B144" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C144" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>264389595</v>
+        <v>267468030</v>
       </c>
       <c r="B145" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>264389599</v>
+        <v>267468034</v>
       </c>
       <c r="B146" t="s">
-        <v>104</v>
+        <v>3</v>
       </c>
       <c r="C146" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Google Sheet autofill new WO
</commit_message>
<xml_diff>
--- a/missed_dates.xlsx
+++ b/missed_dates.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="306">
   <si>
     <t>Work Order Number</t>
   </si>
@@ -31,604 +31,820 @@
     <t>284132439</t>
   </si>
   <si>
-    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5, 8/6</t>
+    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>8/26</t>
+  </si>
+  <si>
+    <t>Hazel</t>
+  </si>
+  <si>
+    <t>284131729</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>8/6, 8/26</t>
+  </si>
+  <si>
+    <t>284131731</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 7/31, 8/1, 8/2, 8/3, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24</t>
+  </si>
+  <si>
+    <t>8/4, 8/18, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131732</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/18, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131733</t>
+  </si>
+  <si>
+    <t>284131734</t>
+  </si>
+  <si>
+    <t>284131735</t>
+  </si>
+  <si>
+    <t>284131737</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/18, 8/20, 8/22, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>8/15, 8/17, 8/19, 8/24</t>
+  </si>
+  <si>
+    <t>284131738</t>
+  </si>
+  <si>
+    <t>7/30</t>
+  </si>
+  <si>
+    <t>8/1, 8/6, 8/8, 8/13, 8/15, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>284131739</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>8/15</t>
+  </si>
+  <si>
+    <t>284131740</t>
+  </si>
+  <si>
+    <t>284131744</t>
+  </si>
+  <si>
+    <t>284131745</t>
+  </si>
+  <si>
+    <t>284131746</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/6</t>
+  </si>
+  <si>
+    <t>284131747</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/19, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>8/18, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131748</t>
+  </si>
+  <si>
+    <t>284131750</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/8, 8/11, 8/13, 8/17, 8/18, 8/20</t>
+  </si>
+  <si>
+    <t>8/6, 8/10, 8/15, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131751</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>8/18, 8/25</t>
+  </si>
+  <si>
+    <t>284131752</t>
+  </si>
+  <si>
+    <t>284131753</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/18, 8/20, 8/22, 8/24, 8/25</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Hazel</t>
-  </si>
-  <si>
-    <t>284131729</t>
-  </si>
-  <si>
-    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5</t>
-  </si>
-  <si>
-    <t>8/6</t>
-  </si>
-  <si>
-    <t>284131731</t>
-  </si>
-  <si>
-    <t>7/29, 7/30, 7/31, 8/1, 8/2, 8/3, 8/5, 8/6, 8/7</t>
+    <t>284131756</t>
+  </si>
+  <si>
+    <t>284131757</t>
+  </si>
+  <si>
+    <t>284131758</t>
+  </si>
+  <si>
+    <t>284131759</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/6, 8/10, 8/13, 8/17, 8/20, 8/24</t>
+  </si>
+  <si>
+    <t>284131760</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>Asphalt Maintenance</t>
+  </si>
+  <si>
+    <t>284131730</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131761</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/10, 8/17, 8/24</t>
+  </si>
+  <si>
+    <t>284131736</t>
+  </si>
+  <si>
+    <t>7/30, 7/31, 8/1, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/18, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/2</t>
+  </si>
+  <si>
+    <t>284131741</t>
+  </si>
+  <si>
+    <t>7/30, 7/31, 8/1, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/17, 8/18, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/2, 8/9, 8/16</t>
+  </si>
+  <si>
+    <t>284131742</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/18, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131764</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/5, 8/11, 8/12, 8/18, 8/24</t>
+  </si>
+  <si>
+    <t>7/29, 8/3, 8/4, 8/6, 8/8, 8/10, 8/13, 8/15, 8/17, 8/19, 8/20, 8/22, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131765</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/19, 8/20, 8/22, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/18</t>
+  </si>
+  <si>
+    <t>284131766</t>
+  </si>
+  <si>
+    <t>8/4, 8/11, 8/18, 8/25</t>
+  </si>
+  <si>
+    <t>284131767</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/20, 8/22, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/19</t>
+  </si>
+  <si>
+    <t>284131768</t>
+  </si>
+  <si>
+    <t>8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/19, 8/20, 8/22, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/3, 8/4, 8/18</t>
+  </si>
+  <si>
+    <t>284131771</t>
+  </si>
+  <si>
+    <t>284131755</t>
+  </si>
+  <si>
+    <t>7/30, 7/31, 8/1, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/17, 8/18, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/2, 8/16</t>
+  </si>
+  <si>
+    <t>284131772</t>
+  </si>
+  <si>
+    <t>284131762</t>
+  </si>
+  <si>
+    <t>8/13, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/15, 8/17, 8/24</t>
+  </si>
+  <si>
+    <t>east coast sweeping</t>
+  </si>
+  <si>
+    <t>284131763</t>
+  </si>
+  <si>
+    <t>8/3, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/4, 8/18, 8/25</t>
+  </si>
+  <si>
+    <t>284131769</t>
+  </si>
+  <si>
+    <t>8/3, 8/6, 8/10, 8/13, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/8, 8/15</t>
+  </si>
+  <si>
+    <t>284131770</t>
+  </si>
+  <si>
+    <t>8/10, 8/13, 8/17, 8/20, 8/24</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/6</t>
+  </si>
+  <si>
+    <t>284131743</t>
+  </si>
+  <si>
+    <t>8/3, 8/5, 8/6, 8/10, 8/12, 8/17, 8/20, 8/24, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/4, 8/8, 8/11, 8/13, 8/15, 8/18, 8/19, 8/22, 8/25</t>
+  </si>
+  <si>
+    <t>Marventanos</t>
+  </si>
+  <si>
+    <t>284131749</t>
+  </si>
+  <si>
+    <t>8/3, 8/5, 8/6, 8/10, 8/12, 8/17, 8/20, 8/24</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/4, 8/8, 8/11, 8/13, 8/15, 8/18, 8/19, 8/22, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131754</t>
+  </si>
+  <si>
+    <t>284131773</t>
+  </si>
+  <si>
+    <t>Madison Group</t>
+  </si>
+  <si>
+    <t>284131774</t>
+  </si>
+  <si>
+    <t>284131775</t>
+  </si>
+  <si>
+    <t>284131776</t>
+  </si>
+  <si>
+    <t>284131777</t>
+  </si>
+  <si>
+    <t>284131778</t>
+  </si>
+  <si>
+    <t>284132179</t>
+  </si>
+  <si>
+    <t>Troiano</t>
+  </si>
+  <si>
+    <t>284132180</t>
+  </si>
+  <si>
+    <t>284132181</t>
+  </si>
+  <si>
+    <t>284132182</t>
+  </si>
+  <si>
+    <t>284132186</t>
+  </si>
+  <si>
+    <t>284131683</t>
+  </si>
+  <si>
+    <t>284132183</t>
+  </si>
+  <si>
+    <t>7/30, 8/6, 8/13</t>
+  </si>
+  <si>
+    <t>8/1, 8/3, 8/8, 8/10, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>By Us ??</t>
+  </si>
+  <si>
+    <t>284132184</t>
+  </si>
+  <si>
+    <t>284132185</t>
+  </si>
+  <si>
+    <t>284131684</t>
+  </si>
+  <si>
+    <t>284132442</t>
+  </si>
+  <si>
+    <t>8/3, 8/10, 8/24</t>
+  </si>
+  <si>
+    <t>7/29, 7/30, 8/1, 8/4, 8/5, 8/6, 8/8, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>Hopwood</t>
+  </si>
+  <si>
+    <t>284131779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GJM </t>
+  </si>
+  <si>
+    <t>284131782</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/15, 8/17, 8/20, 8/24</t>
+  </si>
+  <si>
+    <t>8/22</t>
+  </si>
+  <si>
+    <t>284131787</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29</t>
+  </si>
+  <si>
+    <t>284131791</t>
+  </si>
+  <si>
+    <t>284131798</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>7/29, 8/22, 8/26</t>
+  </si>
+  <si>
+    <t>284131799</t>
+  </si>
+  <si>
+    <t>7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/18, 8/19, 8/20, 8/21, 8/23, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131802</t>
+  </si>
+  <si>
+    <t>284131804</t>
+  </si>
+  <si>
+    <t>284131805</t>
+  </si>
+  <si>
+    <t>284131810</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/18, 8/20, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131812</t>
+  </si>
+  <si>
+    <t>284131813</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/6, 8/8, 8/10, 8/11, 8/12, 8/13, 8/15, 8/17, 8/18, 8/19, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>7/29, 8/26</t>
+  </si>
+  <si>
+    <t>284131685</t>
+  </si>
+  <si>
+    <t>284131686</t>
+  </si>
+  <si>
+    <t>284131687</t>
+  </si>
+  <si>
+    <t>284131688</t>
+  </si>
+  <si>
+    <t>284131689</t>
+  </si>
+  <si>
+    <t>284131693</t>
+  </si>
+  <si>
+    <t>284131694</t>
+  </si>
+  <si>
+    <t>284131695</t>
+  </si>
+  <si>
+    <t>284131696</t>
+  </si>
+  <si>
+    <t>284131697</t>
+  </si>
+  <si>
+    <t>284131698</t>
+  </si>
+  <si>
+    <t>284131699</t>
+  </si>
+  <si>
+    <t>284131728</t>
+  </si>
+  <si>
+    <t>284131780</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/6, 8/10, 8/13, 8/17</t>
+  </si>
+  <si>
+    <t>8/20, 8/24</t>
+  </si>
+  <si>
+    <t>Area Sweeping</t>
+  </si>
+  <si>
+    <t>284131784</t>
+  </si>
+  <si>
+    <t>8/1, 8/3, 8/4, 8/6, 8/8, 8/10, 8/13</t>
+  </si>
+  <si>
+    <t>7/30, 8/11, 8/15, 8/17, 8/18, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131786</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/15</t>
+  </si>
+  <si>
+    <t>8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>284131792</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/10, 8/11, 8/13, 8/17, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>8/15, 8/18</t>
+  </si>
+  <si>
+    <t>284131801</t>
+  </si>
+  <si>
+    <t>284131806</t>
+  </si>
+  <si>
+    <t>284131808</t>
+  </si>
+  <si>
+    <t>8/1, 8/3, 8/6, 8/8, 8/10, 8/13</t>
+  </si>
+  <si>
+    <t>7/30, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>284131781</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/4, 8/5, 8/6, 8/8, 8/11, 8/12, 8/13, 8/15, 8/17, 8/19, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>7/29, 8/3, 8/10, 8/18, 8/26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal </t>
+  </si>
+  <si>
+    <t>284131788</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/4, 8/6, 8/11, 8/13, 8/15, 8/20, 8/22, 8/25</t>
+  </si>
+  <si>
+    <t>8/3, 8/8, 8/10, 8/17, 8/18, 8/24</t>
+  </si>
+  <si>
+    <t>284131793</t>
+  </si>
+  <si>
+    <t>8/4, 8/11, 8/17, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/15, 8/18, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>284131803</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/4, 8/6, 8/8, 8/11, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>8/3, 8/10, 8/18</t>
+  </si>
+  <si>
+    <t>284131700</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/6, 8/13, 8/17, 8/20, 8/24</t>
+  </si>
+  <si>
+    <t>8/10</t>
+  </si>
+  <si>
+    <t>284131701</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>284131702</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>8/10, 8/11, 8/18</t>
+  </si>
+  <si>
+    <t>284131703</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/6, 8/8, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>8/1, 8/10</t>
+  </si>
+  <si>
+    <t>284131704</t>
+  </si>
+  <si>
+    <t>7/30, 7/31, 8/1, 8/2, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>7/29, 8/3, 8/10, 8/18, 8/19, 8/26</t>
+  </si>
+  <si>
+    <t>284131705</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/6, 8/8, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>8/3, 8/10</t>
+  </si>
+  <si>
+    <t>284131714</t>
+  </si>
+  <si>
+    <t>284131783</t>
+  </si>
+  <si>
+    <t>Martorelli</t>
+  </si>
+  <si>
+    <t>284131790</t>
+  </si>
+  <si>
+    <t>8/4, 8/11, 8/18</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/15, 8/17, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131794</t>
+  </si>
+  <si>
+    <t>284131796</t>
+  </si>
+  <si>
+    <t>8/3, 8/4, 8/10, 8/11, 8/17, 8/18, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/6, 8/8, 8/13, 8/15, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>284131797</t>
+  </si>
+  <si>
+    <t>7/30, 8/4, 8/6, 8/11, 8/12, 8/13, 8/18, 8/19, 8/20, 8/25</t>
+  </si>
+  <si>
+    <t>7/29, 8/1, 8/3, 8/5, 8/8, 8/10, 8/15, 8/17, 8/22, 8/24, 8/26</t>
+  </si>
+  <si>
+    <t>284131800</t>
+  </si>
+  <si>
+    <t>284131809</t>
+  </si>
+  <si>
+    <t>7/30, 8/4, 8/5, 8/6, 8/11, 8/12, 8/13, 8/18, 8/19, 8/20, 8/25</t>
+  </si>
+  <si>
+    <t>7/29, 8/1, 8/3, 8/8, 8/10, 8/15, 8/17, 8/22, 8/24, 8/26</t>
+  </si>
+  <si>
+    <t>284131814</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/4, 8/5, 8/6, 8/10, 8/11, 8/12, 8/13, 8/17, 8/18, 8/19, 8/20, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>7/29, 8/1, 8/8, 8/15, 8/22</t>
+  </si>
+  <si>
+    <t>284131817</t>
+  </si>
+  <si>
+    <t>284131785</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17</t>
+  </si>
+  <si>
+    <t>8/4, 8/18, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>284131789</t>
+  </si>
+  <si>
+    <t>284131795</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/18</t>
+  </si>
+  <si>
+    <t>8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131807</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/13, 8/15, 8/17</t>
+  </si>
+  <si>
+    <t>8/20, 8/22, 8/24</t>
+  </si>
+  <si>
+    <t>284131815</t>
+  </si>
+  <si>
+    <t>284131816</t>
+  </si>
+  <si>
+    <t>284131811</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/8, 8/10, 8/13, 8/15, 8/17, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>8/6, 8/24</t>
+  </si>
+  <si>
+    <t>Always Growing</t>
+  </si>
+  <si>
+    <t>284131690</t>
+  </si>
+  <si>
+    <t>Maurice</t>
+  </si>
+  <si>
+    <t>284131692</t>
+  </si>
+  <si>
+    <t>284131691</t>
+  </si>
+  <si>
+    <t>RWN</t>
+  </si>
+  <si>
+    <t>284131706</t>
+  </si>
+  <si>
+    <t>Tom Vangordon/Precision snow</t>
+  </si>
+  <si>
+    <t>284131707</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/3, 8/4, 8/6, 8/8, 8/13, 8/15, 8/22</t>
+  </si>
+  <si>
+    <t>7/29, 8/5, 8/10, 8/11, 8/12, 8/17, 8/18, 8/19, 8/20, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131708</t>
+  </si>
+  <si>
+    <t>7/30, 8/1, 8/4, 8/6, 8/8, 8/13, 8/15, 8/22</t>
+  </si>
+  <si>
+    <t>7/29, 8/3, 8/5, 8/10, 8/11, 8/12, 8/17, 8/18, 8/19, 8/20, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
+    <t>284131711</t>
+  </si>
+  <si>
+    <t>284131712</t>
+  </si>
+  <si>
+    <t>284131713</t>
+  </si>
+  <si>
+    <t>284131717</t>
   </si>
   <si>
     <t>8/4</t>
   </si>
   <si>
-    <t>284131732</t>
-  </si>
-  <si>
-    <t>7/29, 7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/5, 8/6, 8/7</t>
-  </si>
-  <si>
-    <t>284131733</t>
-  </si>
-  <si>
-    <t>284131734</t>
-  </si>
-  <si>
-    <t>284131735</t>
-  </si>
-  <si>
-    <t>284131737</t>
-  </si>
-  <si>
-    <t>284131738</t>
-  </si>
-  <si>
-    <t>7/30</t>
-  </si>
-  <si>
-    <t>8/1, 8/6</t>
-  </si>
-  <si>
-    <t>284131739</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/3, 8/6</t>
-  </si>
-  <si>
-    <t>284131740</t>
-  </si>
-  <si>
-    <t>284131744</t>
-  </si>
-  <si>
-    <t>284131745</t>
-  </si>
-  <si>
-    <t>284131746</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/3, 8/4, 8/5</t>
-  </si>
-  <si>
-    <t>7/29, 8/6</t>
-  </si>
-  <si>
-    <t>284131747</t>
-  </si>
-  <si>
-    <t>284131748</t>
-  </si>
-  <si>
-    <t>284131750</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/3, 8/4</t>
-  </si>
-  <si>
-    <t>284131751</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/3, 8/4, 8/6</t>
-  </si>
-  <si>
-    <t>284131752</t>
-  </si>
-  <si>
-    <t>284131753</t>
-  </si>
-  <si>
-    <t>284131756</t>
-  </si>
-  <si>
-    <t>284131757</t>
-  </si>
-  <si>
-    <t>284131758</t>
-  </si>
-  <si>
-    <t>284131759</t>
-  </si>
-  <si>
-    <t>7/30, 8/3, 8/6</t>
-  </si>
-  <si>
-    <t>284131760</t>
-  </si>
-  <si>
-    <t>Asphalt Maintenance</t>
-  </si>
-  <si>
-    <t>284131730</t>
-  </si>
-  <si>
-    <t>284131761</t>
-  </si>
-  <si>
-    <t>7/30, 8/3</t>
-  </si>
-  <si>
-    <t>284131736</t>
-  </si>
-  <si>
-    <t>7/30, 7/31, 8/1, 8/3, 8/4, 8/5, 8/6, 8/7</t>
-  </si>
-  <si>
-    <t>7/29, 8/2</t>
-  </si>
-  <si>
-    <t>284131741</t>
-  </si>
-  <si>
-    <t>284131742</t>
-  </si>
-  <si>
-    <t>284131764</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/5</t>
-  </si>
-  <si>
-    <t>7/29, 8/3, 8/4, 8/6</t>
-  </si>
-  <si>
-    <t>284131765</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/3, 8/4, 8/5, 8/6</t>
-  </si>
-  <si>
-    <t>7/29</t>
-  </si>
-  <si>
-    <t>284131766</t>
-  </si>
-  <si>
-    <t>284131767</t>
-  </si>
-  <si>
-    <t>284131768</t>
-  </si>
-  <si>
-    <t>8/5, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 7/30, 8/1, 8/3, 8/4</t>
-  </si>
-  <si>
-    <t>284131771</t>
-  </si>
-  <si>
-    <t>284131755</t>
-  </si>
-  <si>
-    <t>284131772</t>
-  </si>
-  <si>
-    <t>284131762</t>
-  </si>
-  <si>
-    <t>east coast sweeping</t>
-  </si>
-  <si>
-    <t>284131763</t>
-  </si>
-  <si>
-    <t>8/3, 8/6</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/4</t>
-  </si>
-  <si>
-    <t>284131769</t>
-  </si>
-  <si>
-    <t>7/30, 8/1</t>
-  </si>
-  <si>
-    <t>284131770</t>
-  </si>
-  <si>
-    <t>284131743</t>
-  </si>
-  <si>
-    <t>8/3, 8/5, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 7/30, 8/1, 8/4</t>
-  </si>
-  <si>
-    <t>Marventanos</t>
-  </si>
-  <si>
-    <t>284131749</t>
-  </si>
-  <si>
-    <t>284131754</t>
-  </si>
-  <si>
-    <t>284131773</t>
-  </si>
-  <si>
-    <t>Madison Group</t>
-  </si>
-  <si>
-    <t>284131774</t>
-  </si>
-  <si>
-    <t>284131775</t>
-  </si>
-  <si>
-    <t>284131776</t>
-  </si>
-  <si>
-    <t>284131777</t>
-  </si>
-  <si>
-    <t>284131778</t>
-  </si>
-  <si>
-    <t>284132179</t>
-  </si>
-  <si>
-    <t>Troiano</t>
-  </si>
-  <si>
-    <t>284132180</t>
-  </si>
-  <si>
-    <t>284132181</t>
-  </si>
-  <si>
-    <t>284132182</t>
-  </si>
-  <si>
-    <t>284132186</t>
-  </si>
-  <si>
-    <t>284131683</t>
-  </si>
-  <si>
-    <t>284132183</t>
-  </si>
-  <si>
-    <t>7/30, 8/6</t>
-  </si>
-  <si>
-    <t>8/1, 8/3</t>
-  </si>
-  <si>
-    <t>By Us ??</t>
-  </si>
-  <si>
-    <t>284132184</t>
-  </si>
-  <si>
-    <t>284132185</t>
-  </si>
-  <si>
-    <t>284131684</t>
-  </si>
-  <si>
-    <t>284132442</t>
-  </si>
-  <si>
-    <t>8/3</t>
-  </si>
-  <si>
-    <t>7/29, 7/30, 8/1, 8/4, 8/5, 8/6</t>
-  </si>
-  <si>
-    <t>Hopwood</t>
-  </si>
-  <si>
-    <t>284131779</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GJM </t>
-  </si>
-  <si>
-    <t>284131782</t>
-  </si>
-  <si>
-    <t>284131787</t>
-  </si>
-  <si>
-    <t>284131791</t>
-  </si>
-  <si>
-    <t>284131798</t>
-  </si>
-  <si>
-    <t>284131799</t>
-  </si>
-  <si>
-    <t>7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/5, 8/6, 8/7</t>
-  </si>
-  <si>
-    <t>284131802</t>
-  </si>
-  <si>
-    <t>284131804</t>
-  </si>
-  <si>
-    <t>284131805</t>
-  </si>
-  <si>
-    <t>284131810</t>
-  </si>
-  <si>
-    <t>284131812</t>
-  </si>
-  <si>
-    <t>284131813</t>
-  </si>
-  <si>
-    <t>284131685</t>
-  </si>
-  <si>
-    <t>284131686</t>
-  </si>
-  <si>
-    <t>284131687</t>
-  </si>
-  <si>
-    <t>284131688</t>
-  </si>
-  <si>
-    <t>284131689</t>
-  </si>
-  <si>
-    <t>284131693</t>
-  </si>
-  <si>
-    <t>284131694</t>
-  </si>
-  <si>
-    <t>284131695</t>
-  </si>
-  <si>
-    <t>284131696</t>
-  </si>
-  <si>
-    <t>284131697</t>
-  </si>
-  <si>
-    <t>284131698</t>
-  </si>
-  <si>
-    <t>284131699</t>
-  </si>
-  <si>
-    <t>284131728</t>
-  </si>
-  <si>
-    <t>284131780</t>
-  </si>
-  <si>
-    <t>Area Sweeping</t>
-  </si>
-  <si>
-    <t>284131784</t>
-  </si>
-  <si>
-    <t>8/1, 8/3, 8/4, 8/6</t>
-  </si>
-  <si>
-    <t>284131786</t>
-  </si>
-  <si>
-    <t>284131792</t>
-  </si>
-  <si>
-    <t>284131801</t>
-  </si>
-  <si>
-    <t>284131806</t>
-  </si>
-  <si>
-    <t>284131808</t>
-  </si>
-  <si>
-    <t>8/1, 8/3, 8/6</t>
-  </si>
-  <si>
-    <t>284131781</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/4, 8/5, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 8/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coastal </t>
-  </si>
-  <si>
-    <t>284131788</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/4, 8/6</t>
-  </si>
-  <si>
-    <t>284131793</t>
-  </si>
-  <si>
-    <t>284131803</t>
-  </si>
-  <si>
-    <t>284131700</t>
-  </si>
-  <si>
-    <t>284131701</t>
-  </si>
-  <si>
-    <t>284131702</t>
-  </si>
-  <si>
-    <t>284131703</t>
-  </si>
-  <si>
-    <t>8/1</t>
-  </si>
-  <si>
-    <t>284131704</t>
-  </si>
-  <si>
-    <t>7/30, 7/31, 8/1, 8/2, 8/4, 8/5, 8/6, 8/7</t>
-  </si>
-  <si>
-    <t>284131705</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/6</t>
-  </si>
-  <si>
-    <t>284131714</t>
-  </si>
-  <si>
-    <t>284131783</t>
-  </si>
-  <si>
-    <t>Martorelli</t>
-  </si>
-  <si>
-    <t>284131790</t>
-  </si>
-  <si>
-    <t>284131794</t>
-  </si>
-  <si>
-    <t>284131796</t>
+    <t>7/30, 8/1, 8/3, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/18, 8/20, 8/22, 8/24, 8/25</t>
+  </si>
+  <si>
+    <t>284131718</t>
   </si>
   <si>
     <t>8/3, 8/4</t>
   </si>
   <si>
-    <t>284131797</t>
-  </si>
-  <si>
-    <t>7/30, 8/4, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 8/1, 8/3, 8/5</t>
-  </si>
-  <si>
-    <t>284131800</t>
-  </si>
-  <si>
-    <t>284131809</t>
-  </si>
-  <si>
-    <t>7/30, 8/4, 8/5, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 8/1, 8/3</t>
-  </si>
-  <si>
-    <t>284131814</t>
-  </si>
-  <si>
-    <t>7/30, 8/3, 8/4, 8/5, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 8/1</t>
-  </si>
-  <si>
-    <t>284131817</t>
-  </si>
-  <si>
-    <t>284131785</t>
-  </si>
-  <si>
-    <t>Split</t>
-  </si>
-  <si>
-    <t>284131789</t>
-  </si>
-  <si>
-    <t>284131795</t>
-  </si>
-  <si>
-    <t>284131807</t>
-  </si>
-  <si>
-    <t>284131815</t>
-  </si>
-  <si>
-    <t>284131816</t>
-  </si>
-  <si>
-    <t>284131811</t>
-  </si>
-  <si>
-    <t>7/30, 8/1, 8/3</t>
-  </si>
-  <si>
-    <t>Always Growing</t>
-  </si>
-  <si>
-    <t>284131690</t>
-  </si>
-  <si>
-    <t>Maurice</t>
-  </si>
-  <si>
-    <t>284131692</t>
-  </si>
-  <si>
-    <t>284131691</t>
-  </si>
-  <si>
-    <t>RWN</t>
-  </si>
-  <si>
-    <t>284131706</t>
-  </si>
-  <si>
-    <t>Tom Vangordon/Precision snow</t>
-  </si>
-  <si>
-    <t>284131707</t>
-  </si>
-  <si>
-    <t>7/29, 8/5</t>
-  </si>
-  <si>
-    <t>284131708</t>
-  </si>
-  <si>
-    <t>7/29, 8/3, 8/5</t>
-  </si>
-  <si>
-    <t>284131711</t>
-  </si>
-  <si>
-    <t>284131712</t>
-  </si>
-  <si>
-    <t>284131713</t>
-  </si>
-  <si>
-    <t>284131717</t>
-  </si>
-  <si>
-    <t>284131718</t>
+    <t>7/30, 8/1, 8/6, 8/8, 8/10, 8/11, 8/13, 8/15, 8/17, 8/18, 8/20, 8/22, 8/24, 8/25</t>
   </si>
   <si>
     <t>284131724</t>
@@ -637,10 +853,10 @@
     <t>284131725</t>
   </si>
   <si>
-    <t>7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/6</t>
-  </si>
-  <si>
-    <t>7/29, 8/5, 8/7</t>
+    <t>7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/6, 8/8, 8/13, 8/14, 8/15, 8/16, 8/21, 8/22, 8/23</t>
+  </si>
+  <si>
+    <t>7/29, 8/5, 8/7, 8/9, 8/10, 8/11, 8/12, 8/17, 8/18, 8/19, 8/20, 8/24, 8/25, 8/26</t>
   </si>
   <si>
     <t>284131726</t>
@@ -655,21 +871,48 @@
     <t>284131710</t>
   </si>
   <si>
+    <t>7/30, 8/13, 8/20</t>
+  </si>
+  <si>
+    <t>8/3, 8/6, 8/10, 8/17, 8/24</t>
+  </si>
+  <si>
     <t>284131715</t>
   </si>
   <si>
+    <t>7/30, 8/1, 8/13, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>8/3, 8/6, 8/8, 8/10, 8/15, 8/17, 8/24</t>
+  </si>
+  <si>
     <t>284131716</t>
   </si>
   <si>
+    <t>7/30, 8/1, 8/6, 8/13, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>8/3, 8/8, 8/10, 8/15, 8/17, 8/24</t>
+  </si>
+  <si>
     <t>284131719</t>
   </si>
   <si>
     <t>284131720</t>
   </si>
   <si>
+    <t>7/30, 8/1, 8/4, 8/11, 8/13, 8/18, 8/20, 8/22</t>
+  </si>
+  <si>
+    <t>8/3, 8/6, 8/8, 8/10, 8/15, 8/17, 8/24, 8/25</t>
+  </si>
+  <si>
     <t>284131721</t>
   </si>
   <si>
+    <t>7/30, 7/31, 8/1, 8/2, 8/3, 8/4, 8/5, 8/6, 8/7, 8/8, 8/9, 8/10, 8/11, 8/12, 8/13, 8/14, 8/15, 8/16, 8/17, 8/18, 8/19, 8/20, 8/21, 8/22, 8/23, 8/24, 8/25, 8/26</t>
+  </si>
+  <si>
     <t>284131722</t>
   </si>
   <si>
@@ -677,6 +920,12 @@
   </si>
   <si>
     <t>284131727</t>
+  </si>
+  <si>
+    <t>7/30, 8/3, 8/6, 8/13, 8/20</t>
+  </si>
+  <si>
+    <t>8/10, 8/17, 8/24</t>
   </si>
   <si>
     <t>Dirtworks</t>
@@ -1184,10 +1433,10 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1195,13 +1444,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1209,13 +1458,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1223,7 +1472,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1237,7 +1486,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1251,7 +1500,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1265,13 +1514,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1279,13 +1528,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1293,7 +1542,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1307,13 +1556,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1321,13 +1570,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1335,13 +1584,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1349,13 +1598,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1363,7 +1612,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -1377,7 +1626,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
         <v>16</v>
@@ -1391,13 +1640,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1405,13 +1654,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1419,156 +1668,156 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" t="s">
         <v>56</v>
-      </c>
-      <c r="D32" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D33" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="E35" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,396 +1825,396 @@
         <v>284117629</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
         <v>68</v>
       </c>
-      <c r="C40" t="s">
-        <v>16</v>
-      </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E50" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E51" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E53" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D54" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E54" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D55" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D58" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E58" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E59" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="E60" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D61" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E61" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D62" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E62" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D63" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E63" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="E64" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C65" t="s">
         <v>16</v>
@@ -1974,49 +2223,49 @@
         <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="C66" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="E66" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C67" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="D67" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C68" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="E68" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2024,130 +2273,130 @@
         <v>281017012</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="D70" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
       <c r="E70" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="D71" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="C72" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="E72" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E73" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="C74" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="D74" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
       <c r="E74" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="C75" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="E75" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="E76" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="C77" t="s">
-        <v>59</v>
+        <v>155</v>
       </c>
       <c r="D77" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="E77" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
@@ -2156,908 +2405,908 @@
         <v>7</v>
       </c>
       <c r="E78" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="C79" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E79" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D80" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E80" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="C81" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E81" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="C82" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D82" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E82" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
       <c r="C83" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E83" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="C84" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E84" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="C85" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D85" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D86" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E86" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="C87" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E87" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="C88" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D88" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E88" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
       <c r="C89" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E89" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D90" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E90" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="C91" t="s">
-        <v>44</v>
+        <v>171</v>
       </c>
       <c r="D91" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="E91" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="C92" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="D92" t="s">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="E92" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="C93" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E93" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="C94" t="s">
-        <v>37</v>
+        <v>181</v>
       </c>
       <c r="D94" t="s">
-        <v>7</v>
+        <v>182</v>
       </c>
       <c r="E94" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="C95" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E95" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="C96" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
       <c r="D96" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E96" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="C97" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="D97" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="E97" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="C98" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="D98" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="E98" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="C99" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="D99" t="s">
-        <v>105</v>
+        <v>194</v>
       </c>
       <c r="E99" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>196</v>
       </c>
       <c r="D100" t="s">
-        <v>25</v>
+        <v>197</v>
       </c>
       <c r="E100" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>152</v>
+        <v>198</v>
       </c>
       <c r="C101" t="s">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="D101" t="s">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="E101" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="C102" t="s">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="D102" t="s">
-        <v>7</v>
+        <v>203</v>
       </c>
       <c r="E102" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="C103" t="s">
-        <v>25</v>
+        <v>205</v>
       </c>
       <c r="D103" t="s">
-        <v>7</v>
+        <v>203</v>
       </c>
       <c r="E103" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
       <c r="C104" t="s">
-        <v>37</v>
+        <v>207</v>
       </c>
       <c r="D104" t="s">
-        <v>7</v>
+        <v>208</v>
       </c>
       <c r="E104" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="C105" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="D105" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
       <c r="E105" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>158</v>
+        <v>212</v>
       </c>
       <c r="C106" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="D106" t="s">
-        <v>147</v>
+        <v>214</v>
       </c>
       <c r="E106" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>160</v>
+        <v>215</v>
       </c>
       <c r="C107" t="s">
-        <v>161</v>
+        <v>216</v>
       </c>
       <c r="D107" t="s">
-        <v>105</v>
+        <v>217</v>
       </c>
       <c r="E107" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
       <c r="C108" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="D108" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
       <c r="E108" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="C109" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="D109" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E109" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>165</v>
+        <v>221</v>
       </c>
       <c r="C110" t="s">
-        <v>14</v>
+        <v>222</v>
       </c>
       <c r="D110" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
       <c r="E110" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>166</v>
+        <v>224</v>
       </c>
       <c r="C111" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="D111" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E111" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>225</v>
       </c>
       <c r="C112" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
       <c r="D112" t="s">
-        <v>161</v>
+        <v>227</v>
       </c>
       <c r="E112" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
       <c r="C113" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
       <c r="D113" t="s">
-        <v>171</v>
+        <v>230</v>
       </c>
       <c r="E113" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
       <c r="C114" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="D114" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E114" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
       <c r="C115" t="s">
-        <v>174</v>
+        <v>233</v>
       </c>
       <c r="D115" t="s">
-        <v>175</v>
+        <v>234</v>
       </c>
       <c r="E115" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="C116" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="D116" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="E116" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="C117" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D117" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E117" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>180</v>
+        <v>239</v>
       </c>
       <c r="C118" t="s">
-        <v>25</v>
+        <v>240</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>241</v>
       </c>
       <c r="E118" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="C119" t="s">
-        <v>44</v>
+        <v>171</v>
       </c>
       <c r="D119" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="E119" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="C120" t="s">
-        <v>37</v>
+        <v>245</v>
       </c>
       <c r="D120" t="s">
-        <v>7</v>
+        <v>246</v>
       </c>
       <c r="E120" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>184</v>
+        <v>247</v>
       </c>
       <c r="C121" t="s">
-        <v>25</v>
+        <v>248</v>
       </c>
       <c r="D121" t="s">
-        <v>7</v>
+        <v>249</v>
       </c>
       <c r="E121" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>185</v>
+        <v>250</v>
       </c>
       <c r="C122" t="s">
-        <v>25</v>
+        <v>248</v>
       </c>
       <c r="D122" t="s">
-        <v>7</v>
+        <v>249</v>
       </c>
       <c r="E122" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="C123" t="s">
-        <v>25</v>
+        <v>248</v>
       </c>
       <c r="D123" t="s">
-        <v>7</v>
+        <v>249</v>
       </c>
       <c r="E123" t="s">
-        <v>181</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>187</v>
+        <v>252</v>
       </c>
       <c r="C124" t="s">
-        <v>188</v>
+        <v>253</v>
       </c>
       <c r="D124" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="E124" t="s">
-        <v>189</v>
+        <v>255</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>190</v>
+        <v>256</v>
       </c>
       <c r="C125" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D125" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E125" t="s">
-        <v>191</v>
+        <v>257</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>192</v>
+        <v>258</v>
       </c>
       <c r="C126" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D126" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E126" t="s">
-        <v>191</v>
+        <v>257</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>193</v>
+        <v>259</v>
       </c>
       <c r="C127" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D127" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E127" t="s">
-        <v>194</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="C128" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D128" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E128" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>197</v>
+        <v>263</v>
       </c>
       <c r="C129" t="s">
-        <v>37</v>
+        <v>264</v>
       </c>
       <c r="D129" t="s">
-        <v>198</v>
+        <v>265</v>
       </c>
       <c r="E129" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>199</v>
+        <v>266</v>
       </c>
       <c r="C130" t="s">
-        <v>150</v>
+        <v>267</v>
       </c>
       <c r="D130" t="s">
-        <v>200</v>
+        <v>268</v>
       </c>
       <c r="E130" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>201</v>
+        <v>269</v>
       </c>
       <c r="C131" t="s">
-        <v>150</v>
+        <v>267</v>
       </c>
       <c r="D131" t="s">
-        <v>200</v>
+        <v>268</v>
       </c>
       <c r="E131" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>202</v>
+        <v>270</v>
       </c>
       <c r="C132" t="s">
-        <v>150</v>
+        <v>267</v>
       </c>
       <c r="D132" t="s">
-        <v>200</v>
+        <v>268</v>
       </c>
       <c r="E132" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>203</v>
+        <v>271</v>
       </c>
       <c r="C133" t="s">
-        <v>37</v>
+        <v>264</v>
       </c>
       <c r="D133" t="s">
-        <v>198</v>
+        <v>265</v>
       </c>
       <c r="E133" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>204</v>
+        <v>272</v>
       </c>
       <c r="C134" t="s">
-        <v>14</v>
+        <v>273</v>
       </c>
       <c r="D134" t="s">
-        <v>25</v>
+        <v>274</v>
       </c>
       <c r="E134" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>205</v>
+        <v>275</v>
       </c>
       <c r="C135" t="s">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="D135" t="s">
-        <v>161</v>
+        <v>277</v>
       </c>
       <c r="E135" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>206</v>
+        <v>278</v>
       </c>
       <c r="C136" t="s">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="D136" t="s">
-        <v>161</v>
+        <v>277</v>
       </c>
       <c r="E136" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
       <c r="C137" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
       <c r="D137" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
       <c r="E137" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>210</v>
+        <v>282</v>
       </c>
       <c r="C138" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D138" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E138" t="s">
-        <v>196</v>
+        <v>262</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>211</v>
+        <v>283</v>
       </c>
       <c r="C139" t="s">
-        <v>177</v>
+        <v>236</v>
       </c>
       <c r="D139" t="s">
-        <v>178</v>
+        <v>237</v>
       </c>
       <c r="E139" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>213</v>
+        <v>285</v>
       </c>
       <c r="C140" t="s">
-        <v>22</v>
+        <v>286</v>
       </c>
       <c r="D140" t="s">
-        <v>72</v>
+        <v>287</v>
       </c>
       <c r="E140" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>214</v>
+        <v>288</v>
       </c>
       <c r="C141" t="s">
-        <v>75</v>
+        <v>289</v>
       </c>
       <c r="D141" t="s">
-        <v>72</v>
+        <v>290</v>
       </c>
       <c r="E141" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>215</v>
+        <v>291</v>
       </c>
       <c r="C142" t="s">
-        <v>161</v>
+        <v>292</v>
       </c>
       <c r="D142" t="s">
-        <v>105</v>
+        <v>293</v>
       </c>
       <c r="E142" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>216</v>
+        <v>294</v>
       </c>
       <c r="C143" t="s">
         <v>16</v>
@@ -3066,77 +3315,77 @@
         <v>7</v>
       </c>
       <c r="E143" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>217</v>
+        <v>295</v>
       </c>
       <c r="C144" t="s">
-        <v>73</v>
+        <v>296</v>
       </c>
       <c r="D144" t="s">
-        <v>72</v>
+        <v>297</v>
       </c>
       <c r="E144" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>218</v>
+        <v>298</v>
       </c>
       <c r="C145" t="s">
-        <v>115</v>
+        <v>299</v>
       </c>
       <c r="D145" t="s">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="E145" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>219</v>
+        <v>300</v>
       </c>
       <c r="C146" t="s">
-        <v>75</v>
+        <v>289</v>
       </c>
       <c r="D146" t="s">
-        <v>72</v>
+        <v>290</v>
       </c>
       <c r="E146" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>220</v>
+        <v>301</v>
       </c>
       <c r="C147" t="s">
-        <v>75</v>
+        <v>289</v>
       </c>
       <c r="D147" t="s">
-        <v>72</v>
+        <v>290</v>
       </c>
       <c r="E147" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>221</v>
+        <v>302</v>
       </c>
       <c r="C148" t="s">
-        <v>44</v>
+        <v>303</v>
       </c>
       <c r="D148" t="s">
-        <v>7</v>
+        <v>304</v>
       </c>
       <c r="E148" t="s">
-        <v>222</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>